<commit_message>
update after receiving the first official Angebot
</commit_message>
<xml_diff>
--- a/Budget KIIWI Projekt V4 - 00.xlsx
+++ b/Budget KIIWI Projekt V4 - 00.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="3" r:id="rId2"/>
-    <sheet name="Mitarbeiter" sheetId="2" r:id="rId3"/>
+    <sheet name="BOM" sheetId="4" r:id="rId3"/>
+    <sheet name="Email.list" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="114">
   <si>
     <t>Number of 
 devices (part)</t>
@@ -79,15 +80,6 @@
   </si>
   <si>
     <t>Raspberry Pi 4B 8 GB</t>
-  </si>
-  <si>
-    <t>tot</t>
-  </si>
-  <si>
-    <t>Hiwi (30 Std/Monat)</t>
-  </si>
-  <si>
-    <t>E10 (40%)</t>
   </si>
   <si>
     <t>Shop I Link</t>
@@ -367,6 +359,141 @@
   </si>
   <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Farnell
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Not-inclTax</t>
+    </r>
+  </si>
+  <si>
+    <t>In our price list inl tax</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Farnel by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>30% estimate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Tax</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Farnel by 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>0% estimate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Tax</t>
+    </r>
+  </si>
+  <si>
+    <t>Batronix</t>
+  </si>
+  <si>
+    <t>fbk-support@kaufland-marketplace.com,kundenmanagement@kaufland.de,impressum@kaufland-online.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaufland </t>
+  </si>
+  <si>
+    <t>Rs-online</t>
+  </si>
+  <si>
+    <t>kunden.service@rs.rsgroup.com, rs-gmbh@rsonline.de, sales@rsonline.ch, bestellung@rs-components.com</t>
+  </si>
+  <si>
+    <t>kundenservice@conrad.de,technical.sales@conrad.de,Businessbetreuung@conrad.de</t>
+  </si>
+  <si>
+    <t>mouser</t>
+  </si>
+  <si>
+    <t>munich.quotes@mouser.com</t>
+  </si>
+  <si>
+    <t>Proshop</t>
+  </si>
+  <si>
+    <t>support@proshop.de, gdpr@proshop.com</t>
+  </si>
+  <si>
+    <t>service @ batronix.com, mail@batronix.com</t>
+  </si>
+  <si>
+    <t>Volkner</t>
+  </si>
+  <si>
+    <t>info@voelkner.de</t>
+  </si>
+  <si>
+    <t>Wucato</t>
+  </si>
+  <si>
+    <t>service@wucato.de</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>030 91588491, sales@digikey.com, eu.support@digikey.com</t>
+  </si>
+  <si>
+    <t>Otto</t>
+  </si>
+  <si>
+    <t>service@otto.de, presse@otto.de</t>
+  </si>
+  <si>
+    <t>Meilhouse.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sales@meilhaus.de,+49 (0) 8141 /5271-0,</t>
+  </si>
+  <si>
+    <t>info@x-kom.de</t>
+  </si>
+  <si>
+    <t>x-com.de</t>
   </si>
 </sst>
 </file>
@@ -468,7 +595,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +617,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,7 +649,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
@@ -705,6 +838,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -970,11 +1136,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="N6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15:XFD15"/>
+      <selection pane="bottomRight" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,10 +1160,10 @@
   <sheetData>
     <row r="1" spans="1:26" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>0</v>
@@ -1005,43 +1171,43 @@
       <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="55"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="81"/>
       <c r="Q1" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="W1" s="10"/>
       <c r="Z1" s="7"/>
@@ -1061,7 +1227,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>3</v>
@@ -1073,16 +1239,16 @@
         <v>5</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P2" s="14" t="s">
         <v>9</v>
@@ -1130,10 +1296,10 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="15"/>
       <c r="R3" s="15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="T3" s="15"/>
       <c r="V3" s="7"/>
@@ -1145,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
@@ -1181,22 +1347,22 @@
         <v>409</v>
       </c>
       <c r="P4" s="44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Q4" s="44" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="S4" s="21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="T4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="V4" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="W4" s="52"/>
       <c r="Z4" s="8"/>
@@ -1237,23 +1403,23 @@
         <v>21.73</v>
       </c>
       <c r="P5" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="T5" s="15"/>
       <c r="U5" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="W5" s="7"/>
       <c r="Z5" s="37"/>
@@ -1263,7 +1429,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" s="8">
         <v>12</v>
@@ -1290,27 +1456,27 @@
       <c r="K6" s="8">
         <v>547.32000000000005</v>
       </c>
-      <c r="O6" s="8">
-        <v>1123.92</v>
+      <c r="O6" s="9">
+        <v>462.36</v>
       </c>
       <c r="P6" s="44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q6" s="31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="R6" s="44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="S6" s="44" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="T6" s="15"/>
       <c r="U6" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="W6" s="8"/>
       <c r="Z6" s="8"/>
@@ -1351,23 +1517,23 @@
         <v>13548.01</v>
       </c>
       <c r="P7" s="33" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q7" s="31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="S7" s="51" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="T7" s="15"/>
       <c r="U7" s="14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="W7" s="7"/>
       <c r="X7" s="19"/>
@@ -1409,23 +1575,23 @@
         <v>5652.5</v>
       </c>
       <c r="P8" s="33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q8" s="31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S8" s="41" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="T8" s="15"/>
       <c r="U8" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="V8" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="W8" s="8"/>
       <c r="Z8" s="8"/>
@@ -1472,22 +1638,22 @@
       </c>
       <c r="P9" s="22"/>
       <c r="Q9" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="S9" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="T9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="S9" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="U9" s="38" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="V9" s="37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W9" s="37"/>
       <c r="Z9" s="37"/>
@@ -1531,29 +1697,29 @@
         <v>870</v>
       </c>
       <c r="N10" s="42" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O10" s="16">
         <v>1105.51</v>
       </c>
       <c r="P10" s="39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q10" s="33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R10" s="39" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="S10" s="39" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="T10" s="39" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="U10" s="18"/>
       <c r="V10" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="W10" s="8"/>
       <c r="Z10" s="8"/>
@@ -1595,17 +1761,17 @@
       </c>
       <c r="P11" s="37"/>
       <c r="Q11" s="31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R11" s="33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S11" s="33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="T11" s="44"/>
       <c r="V11" s="37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="W11" s="37"/>
       <c r="Z11" s="37"/>
@@ -1645,23 +1811,23 @@
         <v>1141.21</v>
       </c>
       <c r="P12" s="33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q12" s="31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="R12" s="41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S12" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="T12" s="41"/>
       <c r="U12" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="V12" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="W12" s="8"/>
       <c r="Z12" s="8"/>
@@ -1707,23 +1873,23 @@
         <v>570</v>
       </c>
       <c r="P13" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="Q13" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="R13" s="41" t="s">
-        <v>37</v>
-      </c>
       <c r="S13" s="50" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="T13" s="41"/>
       <c r="U13" s="45" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="W13" s="7"/>
       <c r="Y13" s="19"/>
@@ -1762,21 +1928,21 @@
         <v>92</v>
       </c>
       <c r="P14" s="33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q14" s="33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="R14" s="31" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
       <c r="U14" s="47" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="V14" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="W14" s="8"/>
       <c r="Z14" s="8"/>
@@ -1823,19 +1989,19 @@
         <v>157</v>
       </c>
       <c r="P15" s="63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q15" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="S15" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="R15" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="S15" s="66" t="s">
-        <v>37</v>
-      </c>
       <c r="T15" s="67" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="V15" s="58"/>
       <c r="W15" s="58"/>
@@ -1844,7 +2010,7 @@
     </row>
     <row r="16" spans="1:26" s="14" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7">
@@ -1860,7 +2026,7 @@
       <c r="K16" s="7"/>
       <c r="O16" s="14">
         <f>SUM(O3:O14)</f>
-        <v>37398.6</v>
+        <v>36737.040000000001</v>
       </c>
       <c r="Q16" s="17"/>
       <c r="R16" s="15"/>
@@ -2057,7 +2223,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="29" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2065,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2073,7 +2239,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2083,43 +2249,344 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C12:G16"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.25" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="1">
-        <f>40*12.41*12</f>
-        <v>5956.7999999999993</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="1">
-        <f>SUM(G1:G13)</f>
-        <v>7446.7999999999993</v>
-      </c>
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" s="69" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="8">
+        <v>12</v>
+      </c>
+      <c r="D3" s="9">
+        <v>462.36</v>
+      </c>
+      <c r="E3" s="16">
+        <v>425.76</v>
+      </c>
+      <c r="F3" s="16">
+        <v>553</v>
+      </c>
+      <c r="G3" s="79"/>
+      <c r="H3" s="16">
+        <f t="shared" ref="H3:H9" si="0">E3 + 0.2*E3</f>
+        <v>510.91199999999998</v>
+      </c>
+      <c r="I3" s="80"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>2</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="37">
+        <v>1</v>
+      </c>
+      <c r="D4" s="37">
+        <v>5652.5</v>
+      </c>
+      <c r="E4" s="73">
+        <v>3325</v>
+      </c>
+      <c r="F4" s="37">
+        <v>4322</v>
+      </c>
+      <c r="H4" s="19">
+        <f t="shared" si="0"/>
+        <v>3990</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="75">
+        <v>2296.6999999999998</v>
+      </c>
+      <c r="E5" s="74">
+        <v>1351</v>
+      </c>
+      <c r="F5" s="16">
+        <v>1756.3</v>
+      </c>
+      <c r="H5" s="16">
+        <f t="shared" si="0"/>
+        <v>1621.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>4</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="37">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19">
+        <v>1105.51</v>
+      </c>
+      <c r="E6" s="19">
+        <v>696.75</v>
+      </c>
+      <c r="F6" s="19">
+        <v>906</v>
+      </c>
+      <c r="H6" s="19">
+        <f t="shared" si="0"/>
+        <v>836.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>5</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>6138.02</v>
+      </c>
+      <c r="E7" s="74">
+        <v>4835.63</v>
+      </c>
+      <c r="F7" s="16">
+        <v>6287</v>
+      </c>
+      <c r="G7" s="80"/>
+      <c r="H7" s="16">
+        <f t="shared" si="0"/>
+        <v>5802.7560000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="70" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>6</v>
+      </c>
+      <c r="B8" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="37">
+        <v>2</v>
+      </c>
+      <c r="D8" s="14">
+        <v>570</v>
+      </c>
+      <c r="E8" s="77">
+        <v>765</v>
+      </c>
+      <c r="F8" s="19">
+        <v>994</v>
+      </c>
+      <c r="G8" s="80"/>
+      <c r="H8" s="19">
+        <f t="shared" si="0"/>
+        <v>918</v>
+      </c>
+      <c r="I8" s="80"/>
+    </row>
+    <row r="9" spans="1:9" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>7</v>
+      </c>
+      <c r="B9" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="78">
+        <v>157</v>
+      </c>
+      <c r="E9" s="16">
+        <v>138.46</v>
+      </c>
+      <c r="F9" s="16">
+        <v>180</v>
+      </c>
+      <c r="G9" s="80"/>
+      <c r="H9" s="16">
+        <f t="shared" si="0"/>
+        <v>166.15200000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for Jonathan enquiries
</commit_message>
<xml_diff>
--- a/Budget KIIWI Projekt V4 - 00.xlsx
+++ b/Budget KIIWI Projekt V4 - 00.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Material" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="BOM2" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="143">
   <si>
     <t>Number of 
 devices (part)</t>
@@ -551,6 +552,18 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Nohau</t>
+  </si>
+  <si>
+    <t>sales@nohau.fi, sales@nohau.se</t>
+  </si>
+  <si>
+    <t>reichelt.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sales@meilhaus.de,+49(0)8141/5271-0,</t>
   </si>
 </sst>
 </file>
@@ -746,7 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
@@ -866,7 +879,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1302,11 +1314,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="P9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,26 +1349,26 @@
       <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108" t="s">
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108" t="s">
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108" t="s">
+      <c r="N1" s="107"/>
+      <c r="O1" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="108"/>
+      <c r="P1" s="107"/>
       <c r="Q1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1512,10 +1524,10 @@
       <c r="O4" s="16">
         <v>409</v>
       </c>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="Q4" s="44" t="s">
+      <c r="Q4" s="43" t="s">
         <v>47</v>
       </c>
       <c r="R4" s="15" t="s">
@@ -1530,7 +1542,7 @@
       <c r="V4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="W4" s="52"/>
+      <c r="W4" s="51"/>
       <c r="Z4" s="8"/>
     </row>
     <row r="5" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1594,7 +1606,7 @@
       <c r="A6" s="16">
         <v>4</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>84</v>
       </c>
       <c r="C6" s="8">
@@ -1625,16 +1637,16 @@
       <c r="O6" s="9">
         <v>462.36</v>
       </c>
-      <c r="P6" s="44" t="s">
+      <c r="P6" s="43" t="s">
         <v>48</v>
       </c>
       <c r="Q6" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="44" t="s">
+      <c r="R6" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="S6" s="44" t="s">
+      <c r="S6" s="43" t="s">
         <v>50</v>
       </c>
       <c r="T6" s="15"/>
@@ -1677,7 +1689,7 @@
         <v>13578.24</v>
       </c>
       <c r="K7" s="7">
-        <v>1294</v>
+        <v>15528</v>
       </c>
       <c r="O7" s="7">
         <v>13548.01</v>
@@ -1691,7 +1703,7 @@
       <c r="R7" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="S7" s="51" t="s">
+      <c r="S7" s="50" t="s">
         <v>80</v>
       </c>
       <c r="T7" s="15"/>
@@ -1809,7 +1821,7 @@
       <c r="R9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="S9" s="43" t="s">
+      <c r="S9" s="50" t="s">
         <v>27</v>
       </c>
       <c r="T9" s="6" t="s">
@@ -1935,7 +1947,7 @@
       <c r="S11" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="T11" s="44"/>
+      <c r="T11" s="43"/>
       <c r="V11" s="37" t="s">
         <v>66</v>
       </c>
@@ -2055,11 +2067,11 @@
       <c r="R13" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="S13" s="50" t="s">
+      <c r="S13" s="49" t="s">
         <v>82</v>
       </c>
       <c r="T13" s="41"/>
-      <c r="U13" s="45" t="s">
+      <c r="U13" s="44" t="s">
         <v>68</v>
       </c>
       <c r="V13" s="7" t="s">
@@ -2073,7 +2085,7 @@
       <c r="A14" s="16">
         <v>12</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="8">
@@ -2097,7 +2109,7 @@
         <v>92</v>
       </c>
       <c r="K14" s="8"/>
-      <c r="N14" s="46"/>
+      <c r="N14" s="45"/>
       <c r="O14" s="16">
         <v>92</v>
       </c>
@@ -2112,7 +2124,7 @@
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
-      <c r="U14" s="47" t="s">
+      <c r="U14" s="46" t="s">
         <v>71</v>
       </c>
       <c r="V14" s="8" t="s">
@@ -2121,66 +2133,66 @@
       <c r="W14" s="8"/>
       <c r="Z14" s="8"/>
     </row>
-    <row r="15" spans="1:26" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="56">
+    <row r="15" spans="1:26" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="55">
         <v>13</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="58">
+      <c r="C15" s="57">
         <v>2</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="57">
         <v>232.57</v>
       </c>
-      <c r="E15" s="58">
+      <c r="E15" s="57">
         <v>89.94</v>
       </c>
-      <c r="F15" s="58">
+      <c r="F15" s="57">
         <v>95.8</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="57">
         <v>84.99</v>
       </c>
-      <c r="H15" s="58">
+      <c r="H15" s="57">
         <v>78.5</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="57">
         <v>169.98</v>
       </c>
-      <c r="J15" s="58">
+      <c r="J15" s="57">
         <v>191.6</v>
       </c>
-      <c r="K15" s="59">
+      <c r="K15" s="58">
         <v>169.98</v>
       </c>
-      <c r="L15" s="60">
+      <c r="L15" s="59">
         <v>157</v>
       </c>
-      <c r="M15" s="61"/>
-      <c r="O15" s="62">
+      <c r="M15" s="60"/>
+      <c r="O15" s="61">
         <v>157</v>
       </c>
-      <c r="P15" s="63" t="s">
+      <c r="P15" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="64" t="s">
+      <c r="Q15" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="R15" s="65" t="s">
+      <c r="R15" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="S15" s="66" t="s">
+      <c r="S15" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="T15" s="67" t="s">
+      <c r="T15" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="V15" s="58"/>
-      <c r="W15" s="58"/>
-      <c r="Y15" s="68"/>
-      <c r="Z15" s="58"/>
+      <c r="V15" s="57"/>
+      <c r="W15" s="57"/>
+      <c r="Y15" s="67"/>
+      <c r="Z15" s="57"/>
     </row>
     <row r="16" spans="1:26" s="14" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
@@ -2403,7 +2415,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="29" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48">
+      <c r="A2" s="47">
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
@@ -2411,7 +2423,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="49">
+      <c r="A3" s="48">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -2425,10 +2437,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,7 +2457,7 @@
       <c r="A2" t="s">
         <v>89</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="50" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2525,13 +2537,41 @@
       <c r="A12" t="s">
         <v>108</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="50" t="s">
         <v>107</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B12" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2539,7 +2579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2559,43 +2599,43 @@
       <c r="B1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="82"/>
-      <c r="H1" s="78" t="s">
+      <c r="G1" s="81"/>
+      <c r="H1" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="88" t="s">
+      <c r="I1" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="J1" s="88" t="s">
+      <c r="J1" s="87" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="79"/>
-    </row>
-    <row r="3" spans="1:11" s="69" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="78"/>
+    </row>
+    <row r="3" spans="1:11" s="68" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>4</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>84</v>
       </c>
       <c r="C3" s="8">
@@ -2607,15 +2647,15 @@
       <c r="E3" s="16">
         <v>425.76</v>
       </c>
-      <c r="F3" s="80">
+      <c r="F3" s="79">
         <v>553</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="80">
+      <c r="G3" s="82"/>
+      <c r="H3" s="79">
         <f t="shared" ref="H3:H9" si="0">E3 + 0.2*E3</f>
         <v>510.91199999999998</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="I3" s="76" t="s">
         <v>109</v>
       </c>
       <c r="J3" s="16">
@@ -2635,23 +2675,23 @@
       <c r="D4" s="37">
         <v>5652.5</v>
       </c>
-      <c r="E4" s="73">
+      <c r="E4" s="72">
         <v>3325</v>
       </c>
-      <c r="F4" s="81">
+      <c r="F4" s="80">
         <v>4322</v>
       </c>
-      <c r="G4" s="82"/>
-      <c r="H4" s="79">
+      <c r="G4" s="81"/>
+      <c r="H4" s="78">
         <f t="shared" si="0"/>
         <v>3990</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="86">
         <v>8358.07</v>
       </c>
-      <c r="J4" s="77"/>
-    </row>
-    <row r="5" spans="1:11" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="76"/>
+    </row>
+    <row r="5" spans="1:11" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>7</v>
       </c>
@@ -2661,24 +2701,24 @@
       <c r="C5" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="74">
         <v>2296.6999999999998</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E5" s="73">
         <v>1351</v>
       </c>
-      <c r="F5" s="80">
+      <c r="F5" s="79">
         <v>1756.3</v>
       </c>
-      <c r="G5" s="84"/>
-      <c r="H5" s="80">
+      <c r="G5" s="83"/>
+      <c r="H5" s="79">
         <f t="shared" si="0"/>
         <v>1621.2</v>
       </c>
       <c r="I5" s="16">
         <v>1639.71</v>
       </c>
-      <c r="J5" s="77"/>
+      <c r="J5" s="76"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
@@ -2696,20 +2736,20 @@
       <c r="E6" s="19">
         <v>696.75</v>
       </c>
-      <c r="F6" s="79">
+      <c r="F6" s="78">
         <v>906</v>
       </c>
-      <c r="G6" s="82"/>
-      <c r="H6" s="79">
+      <c r="G6" s="81"/>
+      <c r="H6" s="78">
         <f t="shared" si="0"/>
         <v>836.1</v>
       </c>
       <c r="I6" s="14">
         <v>751.33</v>
       </c>
-      <c r="J6" s="77"/>
-    </row>
-    <row r="7" spans="1:11" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="76"/>
+    </row>
+    <row r="7" spans="1:11" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>9</v>
       </c>
@@ -2722,27 +2762,27 @@
       <c r="D7" s="8">
         <v>6138.02</v>
       </c>
-      <c r="E7" s="74">
+      <c r="E7" s="73">
         <v>4835.63</v>
       </c>
-      <c r="F7" s="80">
+      <c r="F7" s="79">
         <v>6287</v>
       </c>
-      <c r="G7" s="85"/>
-      <c r="H7" s="80">
+      <c r="G7" s="84"/>
+      <c r="H7" s="79">
         <f t="shared" si="0"/>
         <v>5802.7560000000003</v>
       </c>
       <c r="I7" s="16">
         <v>5158</v>
       </c>
-      <c r="J7" s="77"/>
-    </row>
-    <row r="8" spans="1:11" s="70" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7" s="76"/>
+    </row>
+    <row r="8" spans="1:11" s="69" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>11</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="71" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="37">
@@ -2751,43 +2791,43 @@
       <c r="D8" s="14">
         <v>570</v>
       </c>
-      <c r="E8" s="95">
+      <c r="E8" s="94">
         <v>765</v>
       </c>
-      <c r="F8" s="79">
+      <c r="F8" s="78">
         <v>994</v>
       </c>
-      <c r="G8" s="85"/>
-      <c r="H8" s="91">
+      <c r="G8" s="84"/>
+      <c r="H8" s="90">
         <f t="shared" si="0"/>
         <v>918</v>
       </c>
       <c r="I8" s="19">
         <v>411.48</v>
       </c>
-      <c r="J8" s="77"/>
-    </row>
-    <row r="9" spans="1:11" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="76"/>
+    </row>
+    <row r="9" spans="1:11" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>13</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="70" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="8">
         <v>2</v>
       </c>
-      <c r="D9" s="106">
+      <c r="D9" s="105">
         <v>157</v>
       </c>
       <c r="E9" s="16">
         <v>138.46</v>
       </c>
-      <c r="F9" s="80">
+      <c r="F9" s="79">
         <v>180</v>
       </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="80">
+      <c r="G9" s="84"/>
+      <c r="H9" s="79">
         <f t="shared" si="0"/>
         <v>166.15200000000002</v>
       </c>
@@ -2798,41 +2838,41 @@
         <v>142.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="105" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="102">
+    <row r="10" spans="1:11" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="101">
         <v>10</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="104">
+      <c r="C10" s="103">
         <v>1</v>
       </c>
-      <c r="D10" s="105">
+      <c r="D10" s="104">
         <v>1141.21</v>
       </c>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="I10" s="102"/>
-      <c r="J10" s="102">
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101">
         <v>1049.75</v>
       </c>
-      <c r="K10" s="105" t="s">
+      <c r="K10" s="104" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="93" t="s">
+    <row r="11" spans="1:11" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="94">
+      <c r="E11" s="93">
         <v>7</v>
       </c>
-      <c r="F11" s="94"/>
-      <c r="I11" s="94">
+      <c r="F11" s="93"/>
+      <c r="I11" s="93">
         <v>6</v>
       </c>
-      <c r="J11" s="94">
+      <c r="J11" s="93">
         <v>3</v>
       </c>
     </row>
@@ -2872,68 +2912,68 @@
       <c r="B14" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="76">
+      <c r="D14" s="75">
         <f>SUM(D3:D9)</f>
         <v>16382.09</v>
       </c>
-      <c r="E14" s="92">
+      <c r="E14" s="91">
         <v>13729.74</v>
       </c>
-      <c r="I14" s="92">
+      <c r="I14" s="91">
         <v>19589.099999999999</v>
       </c>
-      <c r="J14" s="49">
+      <c r="J14" s="48">
         <v>1969</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="99" t="s">
+    <row r="16" spans="1:11" s="98" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="98" t="s">
         <v>119</v>
       </c>
-      <c r="D16" s="100"/>
-      <c r="E16" s="101">
+      <c r="D16" s="99"/>
+      <c r="E16" s="100">
         <f>E14-D14</f>
         <v>-2652.3500000000004</v>
       </c>
-      <c r="F16" s="101"/>
-      <c r="I16" s="101">
+      <c r="F16" s="100"/>
+      <c r="I16" s="100">
         <f>I14-D14</f>
         <v>3207.0099999999984</v>
       </c>
-      <c r="J16" s="101"/>
+      <c r="J16" s="100"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>120</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="I17" s="51" t="s">
+      <c r="I17" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="J17" s="51" t="s">
+      <c r="J17" s="50" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="98"/>
-      <c r="B22" s="107" t="s">
+      <c r="A22" s="97"/>
+      <c r="B22" s="106" t="s">
         <v>138</v>
       </c>
       <c r="C22" t="s">
         <v>129</v>
       </c>
-      <c r="G22" s="98">
+      <c r="G22" s="97">
         <v>578.34</v>
       </c>
       <c r="H22" t="s">
         <v>130</v>
       </c>
-      <c r="J22" s="51" t="s">
+      <c r="J22" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="K22" s="51" t="s">
+      <c r="K22" s="50" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2954,14 +2994,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="14"/>
-    <col min="2" max="2" width="14.25" style="96" customWidth="1"/>
+    <col min="2" max="2" width="14.25" style="95" customWidth="1"/>
     <col min="3" max="5" width="9" style="14"/>
   </cols>
   <sheetData>
@@ -2981,10 +3021,10 @@
       <c r="E1" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="88" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2992,7 +3032,7 @@
       <c r="A3" s="14">
         <v>5</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="95" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="14">
@@ -3005,7 +3045,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="70" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="69" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>10</v>
       </c>
@@ -3015,7 +3055,7 @@
       <c r="C4" s="37">
         <v>1</v>
       </c>
-      <c r="D4" s="70">
+      <c r="D4" s="69">
         <v>1141.21</v>
       </c>
       <c r="E4" s="19"/>
@@ -3029,23 +3069,23 @@
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
     </row>
-    <row r="5" spans="1:10" s="93" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="97" t="s">
+    <row r="5" spans="1:10" s="92" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="94">
+      <c r="E5" s="93">
         <v>7</v>
       </c>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94">
+      <c r="F5" s="93"/>
+      <c r="G5" s="93">
         <v>1</v>
       </c>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="93"/>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6"/>
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="89" t="s">
         <v>112</v>
       </c>
       <c r="C6"/>
@@ -3057,7 +3097,7 @@
       <c r="G6">
         <v>1049.75</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="48">
         <v>959</v>
       </c>
       <c r="I6" s="14"/>
@@ -3065,7 +3105,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7"/>
-      <c r="B7" s="90" t="s">
+      <c r="B7" s="89" t="s">
         <v>113</v>
       </c>
       <c r="C7"/>
@@ -3079,7 +3119,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8"/>
-      <c r="B8" s="90" t="s">
+      <c r="B8" s="89" t="s">
         <v>114</v>
       </c>
       <c r="C8"/>
@@ -3102,7 +3142,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9"/>
-      <c r="B9" s="90"/>
+      <c r="B9" s="89"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="F9" s="14"/>
@@ -3111,7 +3151,7 @@
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10"/>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="89" t="s">
         <v>119</v>
       </c>
       <c r="C10"/>
@@ -3126,20 +3166,20 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11"/>
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="89" t="s">
         <v>120</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="50" t="s">
         <v>128</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="H11" s="51" t="s">
+      <c r="H11" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>